<commit_message>
starting to save cryptocurrency data in an excel sheet
</commit_message>
<xml_diff>
--- a/Data/criptomoedas.xlsx
+++ b/Data/criptomoedas.xlsx
@@ -1,24 +1,52 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
+    <sheet name="Cripto" sheetId="1" r:id="rId1"/>
     <sheet name="Plan2" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+  <si>
+    <t>Criptomoeda</t>
+  </si>
+  <si>
+    <t>Valor da última consulta</t>
+  </si>
+  <si>
+    <t>Valor do dia atual</t>
+  </si>
+  <si>
+    <t>% de aumento</t>
+  </si>
+  <si>
+    <t>% de queda</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -46,21 +74,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Escritório">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -98,7 +132,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Escritório">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -170,7 +204,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Escritório">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -343,36 +377,64 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Checking if Crypto exists in excel sheet
</commit_message>
<xml_diff>
--- a/Data/criptomoedas.xlsx
+++ b/Data/criptomoedas.xlsx
@@ -1,94 +1,125 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Cripto" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="122211"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Cripto" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Plan3" sheetId="3" r:id="rId3"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="122211"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Criptomoeda</t>
-  </si>
-  <si>
-    <t>Valor da última consulta</t>
-  </si>
-  <si>
-    <t>Valor do dia atual</t>
-  </si>
-  <si>
-    <t>% de aumento</t>
-  </si>
-  <si>
-    <t>% de queda</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <x:si>
+    <x:t>Criptomoeda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor da última consulta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor do dia atual</x:t>
+  </x:si>
+  <x:si>
+    <x:t>% de aumento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>% de queda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bitcoin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>$31,398.61</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="5">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,65 +408,93 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E1"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="C2" sqref="C2 C2:C2"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="12.570312" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="22.710938" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="16.570312" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="13.855469" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="11.285156" style="3" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="4" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="4" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5">
+      <x:c r="A2" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
adding data to excel file
</commit_message>
<xml_diff>
--- a/Data/criptomoedas.xlsx
+++ b/Data/criptomoedas.xlsx
@@ -1,95 +1,140 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Cripto" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="122211"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Cripto" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Plan3" sheetId="3" r:id="rId3"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="122211"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Criptomoeda</t>
-  </si>
-  <si>
-    <t>Valor da última consulta</t>
-  </si>
-  <si>
-    <t>Valor do dia atual</t>
-  </si>
-  <si>
-    <t>% de aumento</t>
-  </si>
-  <si>
-    <t>% de queda</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+  <x:si>
+    <x:t>Criptomoeda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor Atual</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor Última Consulta</x:t>
+  </x:si>
+  <x:si>
+    <x:t>% de aumento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>% de queda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bitcoin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30.242,9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ethereum</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.792,04</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dogecoin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,079419</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,079529</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="5">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,65 +423,121 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E4"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="A6" sqref="A6 A6:A6"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="12.570312" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="22.710938" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="20.570312" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="13.855469" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="11.285156" style="3" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="4" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="4" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="B3" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A4" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E4" s="3" t="s"/>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B5" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="3" t="s"/>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
Add data file excel
</commit_message>
<xml_diff>
--- a/Data/criptomoedas.xlsx
+++ b/Data/criptomoedas.xlsx
@@ -1,95 +1,146 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Cripto" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
-  </sheets>
-  <calcPr calcId="122211"/>
-</workbook>
+<x:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <x:fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+  <x:workbookPr filterPrivacy="1" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <x:bookViews>
+    <x:workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="0" activeTab="0"/>
+  </x:bookViews>
+  <x:sheets>
+    <x:sheet name="Cripto" sheetId="1" r:id="rId1"/>
+    <x:sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <x:sheet name="Plan3" sheetId="3" r:id="rId3"/>
+  </x:sheets>
+  <x:definedNames/>
+  <x:calcPr calcId="122211"/>
+</x:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>Criptomoeda</t>
-  </si>
-  <si>
-    <t>% de aumento</t>
-  </si>
-  <si>
-    <t>% de queda</t>
-  </si>
-  <si>
-    <t>Valor Atual</t>
-  </si>
-  <si>
-    <t>Valor Anterior</t>
-  </si>
-</sst>
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <x:si>
+    <x:t>Criptomoeda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor Atual</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Valor Anterior</x:t>
+  </x:si>
+  <x:si>
+    <x:t>% de aumento</x:t>
+  </x:si>
+  <x:si>
+    <x:t>% de queda</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bitcoin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29.923,4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29.778,5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Ethereum</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.777,76</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.775,13</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Dogecoin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,079035</x:t>
+  </x:si>
+  <x:si>
+    <x:t>0,078967</x:t>
+  </x:si>
+</x:sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-  </fonts>
-  <fills count="2">
-    <fill>
-      <patternFill patternType="none"/>
-    </fill>
-    <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-  </fills>
-  <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-  </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
-  </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+<x:styleSheet xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:numFmts count="1">
+    <x:numFmt numFmtId="0" formatCode=""/>
+  </x:numFmts>
+  <x:fonts count="3" x14ac:knownFonts="1">
+    <x:font>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:b/>
+      <x:sz val="11"/>
+      <x:color theme="1"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+      <x:scheme val="minor"/>
+    </x:font>
+    <x:font>
+      <x:vertAlign val="baseline"/>
+      <x:sz val="11"/>
+      <x:color rgb="FF000000"/>
+      <x:name val="Calibri"/>
+      <x:family val="2"/>
+    </x:font>
+  </x:fonts>
+  <x:fills count="2">
+    <x:fill>
+      <x:patternFill patternType="none"/>
+    </x:fill>
+    <x:fill>
+      <x:patternFill patternType="gray125"/>
+    </x:fill>
+  </x:fills>
+  <x:borders count="1">
+    <x:border>
+      <x:left/>
+      <x:right/>
+      <x:top/>
+      <x:bottom/>
+      <x:diagonal/>
+    </x:border>
+  </x:borders>
+  <x:cellStyleXfs count="3">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellStyleXfs>
+  <x:cellXfs count="5">
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <x:xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+    <x:xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="1">
+      <x:alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <x:protection locked="1" hidden="0"/>
+    </x:xf>
+  </x:cellXfs>
+  <x:cellStyles count="1">
+    <x:cellStyle name="Normal" xfId="0" builtinId="0"/>
+  </x:cellStyles>
+  <x:tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <x:extLst>
+    <x:ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
-</styleSheet>
+    </x:ext>
+  </x:extLst>
+</x:styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -378,65 +429,119 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1:E3"/>
+  <x:sheetViews>
+    <x:sheetView tabSelected="1" workbookViewId="0">
+      <x:selection activeCell="B4" sqref="B4 B4:B4"/>
+    </x:sheetView>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:cols>
+    <x:col min="1" max="1" width="12.570312" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="2" max="2" width="10.855469" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="3" max="3" width="13.710938" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="4" max="4" width="13.855469" style="3" bestFit="1" customWidth="1"/>
+    <x:col min="5" max="5" width="11.285156" style="3" bestFit="1" customWidth="1"/>
+  </x:cols>
+  <x:sheetData>
+    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A1" s="4" t="s">
+        <x:v>0</x:v>
+      </x:c>
+      <x:c r="B1" s="4" t="s">
+        <x:v>1</x:v>
+      </x:c>
+      <x:c r="C1" s="4" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D1" s="4" t="s">
+        <x:v>3</x:v>
+      </x:c>
+      <x:c r="E1" s="4" t="s">
+        <x:v>4</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A2" s="3" t="s">
+        <x:v>5</x:v>
+      </x:c>
+      <x:c r="B2" s="3" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="C2" s="3" t="s">
+        <x:v>7</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <x:c r="A3" s="3" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B3" s="3" t="s">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="C3" s="3" t="s">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="E3" s="3" t="s"/>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="3" t="s">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B4" s="3" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="C4" s="3" t="s">
+        <x:v>13</x:v>
+      </x:c>
+    </x:row>
+  </x:sheetData>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="9" scale="100" pageOrder="downThenOver" orientation="portrait" blackAndWhite="0" draft="0" cellComments="none" errors="displayed" r:id="rId1"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
+<x:worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x14ac">
+  <x:sheetPr>
+    <x:outlinePr summaryBelow="1" summaryRight="1"/>
+  </x:sheetPr>
+  <x:dimension ref="A1"/>
+  <x:sheetViews>
+    <x:sheetView workbookViewId="0"/>
+  </x:sheetViews>
+  <x:sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <x:sheetData/>
+  <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
+  <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <x:pageSetup paperSize="1" scale="100" pageOrder="downThenOver" orientation="default" blackAndWhite="0" draft="0" cellComments="none" errors="displayed"/>
+  <x:headerFooter/>
+  <x:tableParts count="0"/>
+</x:worksheet>
 </file>
</xml_diff>

<commit_message>
crypto fall in value calculation
</commit_message>
<xml_diff>
--- a/Data/criptomoedas.xlsx
+++ b/Data/criptomoedas.xlsx
@@ -37,10 +37,10 @@
     <x:t>Bitcoin</x:t>
   </x:si>
   <x:si>
-    <x:t>29.923,4</x:t>
-  </x:si>
-  <x:si>
-    <x:t>29.778,5</x:t>
+    <x:t>30.027,0</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30.023,1</x:t>
   </x:si>
   <x:si>
     <x:t>Ethereum</x:t>

</xml_diff>

<commit_message>
calculating percentage of fall
</commit_message>
<xml_diff>
--- a/Data/criptomoedas.xlsx
+++ b/Data/criptomoedas.xlsx
@@ -37,28 +37,28 @@
     <x:t>Bitcoin</x:t>
   </x:si>
   <x:si>
-    <x:t>30.027,0</x:t>
-  </x:si>
-  <x:si>
-    <x:t>30.023,1</x:t>
+    <x:t>28.497,8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>28.446,1</x:t>
   </x:si>
   <x:si>
     <x:t>Ethereum</x:t>
   </x:si>
   <x:si>
-    <x:t>1.777,76</x:t>
-  </x:si>
-  <x:si>
-    <x:t>1.775,13</x:t>
+    <x:t>1.537,2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>1.525,38</x:t>
   </x:si>
   <x:si>
     <x:t>Dogecoin</x:t>
   </x:si>
   <x:si>
+    <x:t>0,069827</x:t>
+  </x:si>
+  <x:si>
     <x:t>0,079035</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0,078967</x:t>
   </x:si>
 </x:sst>
 </file>

</xml_diff>